<commit_message>
Giải thích về phúc đức các sao chính
</commit_message>
<xml_diff>
--- a/LuanPhucDuc.xlsx
+++ b/LuanPhucDuc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10FC46D-66C1-4211-84FC-3E8123197B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEB9A2D-85E9-484C-8E4F-2DD4B190D64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5355" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8752" uniqueCount="4411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8756" uniqueCount="4437">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13172,17 +13172,10 @@
     <t>Được hưởng phúc. Trong họ ít của, hiếm người.</t>
   </si>
   <si>
-    <t>Suốt đời sung sướng, phúc thọ song toàn. Trong họ có
-nhiều người giàu sang.</t>
-  </si>
-  <si>
     <t>Được hưởng phúc. Họ hàng khá giả nhưng hiếm người.</t>
   </si>
   <si>
     <t xml:space="preserve">Vất vả lao khổ, phải xa quê hương mới sống lâu. Họ hàng ly tán. </t>
-  </si>
-  <si>
-    <t>Giảm thọ, khó tránh được tai ương, họa hại. Trong họ có nhiều người bần hàn hay mắc tù tội, thường phải bạt quán xiêu cư.</t>
   </si>
   <si>
     <t>Giảm thọ, hay gặp nguy hiểm, phải xa quê hương mới mong được an toàn. Trong họ có nhiều người chết non một cách thê thảm. Nếu không, cũng phải mang tàn tật, ác bệnh, hay mắc tù tội, khốn cùng.</t>
@@ -13268,6 +13261,98 @@
   </si>
   <si>
     <t>Không được hưởng phúc dồi dào nên suốt đời chẳng được xứng ý toại lòng. Họ hàng bình thường,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Được hưởng phúc, sống lâu. Họ hàng đông đảo, khá
+giả </t>
+  </si>
+  <si>
+    <t>Không được hưởng phúc dồi dào. Nên lập nghiệp ở nơi thật xa quê hương. Trong họ, nhiều người giàu sang, nhưng ly tán.</t>
+  </si>
+  <si>
+    <t>Thiên Phủ đồng cung với Thiên Tướng tại Phúc Đức</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suốt đời được xứng ý toại lòng, sống lâu và hưởng phúc. Họ hàng nhiều người giàu sang. </t>
+  </si>
+  <si>
+    <t>Suốt đời sung sướng, phúc thọ song toàn. Trong họ có nhiều người giàu sang.</t>
+  </si>
+  <si>
+    <t>Được hưởng phúc trọn đời, sung sướng, sống lâu. Trong họ có nhiều người qúy hiến và giàu sang.</t>
+  </si>
+  <si>
+    <t>Bạc phúc nên tuổi thọ bị chiết giảm. Suốt đời vui ít buồn nhiều, lao tâm khổ tứ. Nên lập nghiệp ở nơi thật xa quê hương, có sớm xa cách gia đình mới mong được yên thân. Họ hàng ly tán, nhiều người cùng khổ, cô đơn, mang ác tật, phiêu bạt giang hồ, hay mắc tai nạn mà chết một cách thê thảm. Đàn bà con gái trong họ rất vất vả về chồng con.</t>
+  </si>
+  <si>
+    <t>Được hưởng phúc. Về già rất sung sướng. Trong họ nhiều người giàu có, nhưng thường lập nghiệp ở nơi thật xa quê hương.</t>
+  </si>
+  <si>
+    <t>Không được hưởng phúc dồi dào, nhưng cũng sống lâu. Họ hàng bình thường, có nhiều người lập thân bằng võ nghiệp.</t>
+  </si>
+  <si>
+    <t>Bạc phúc nên giảm thọ. Phải lập nghiệp ở xa quê
+hương, phải sớm xa gia đình mới mong được yên thân. Họ hàng ly tán, càng ngày càng sa sút, lại có nhiều người rất dâm đãng</t>
+  </si>
+  <si>
+    <t>Giảm thọ, khó tránh được tai ương, họa hại. Trong họ có nhiều người bần hàn hay mắc tù tội, thường phải phiêu bạt nay đây mai đó.</t>
+  </si>
+  <si>
+    <t>Được hưởng phúc, sống lâu, về già rất sung sướng. Họ hàng giàu có qúy hiển</t>
+  </si>
+  <si>
+    <t>Giảm thọ. Suốt đời lao tâm khổ tứ chẳng được xứng ý toại lòng, lại hay mắc tai nạn khẩu thiệt, kiện cáo. Phải sớm xa gia đình mới mong được yên thân. Trong họ thường có sự tranh chấp, nhiều người phải bỏ quê xa xứ, nếu không, cũng khốn cùng, mắc hình ngục, hay yểu tử.</t>
+  </si>
+  <si>
+    <t>Được hưởng phúc, sống lâu và sung sướng. Họ hàng qúy hiển, giàu sang, có danh giá và uy quyền tế thế.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Được hưởng phúc, suốt đời bay gặp may mắn. Trong họ có nhiều người qúy hiển, giàu sang. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Không được hưởng phúc dồi dào, nên lúc thiếu thời
+chẳng được xứng ý toại lòng. Về già hay gặp may mắn. Họ hàng càng ngày càng khá giả. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Được hưởng phúc, thanh nhàn, sung sướng tránh
+được nhiều tai họa và sống lâu. Trong họ có nhiều người qúy hiến, có danh tiếng lừng lẫy. </t>
+  </si>
+  <si>
+    <t>Được hưởng phúc, sống lâu. Họ hàng bình thường.</t>
+  </si>
+  <si>
+    <t>Giảm thọ, khó tránh được tai họa. thường phải sớm
+xa gia đình, nay đây mai đó, hay thay đổi công việc và chí hướng. Họ hàng càng ngày càng sa sút ly tán, đàn ông con trai có nhiều người chơi bời, du đãng, đàn
+bà con gái cũng có nhiều người dâm dật, hay trắc trở về chồng con</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạc phúc nên tuổi thọ bị chiết giảm. Suốt đời chẳng được xứng ý toại lòng. Nên ly tổ hay ở xa gia đình. Họ hàng càng ngày càng sa sút ly tán, có nhiều người gian quyệt nhưng bần cùng, có người phiêu bạt giang hồ, lại có người mang ác tật hay mắc tai nạn chết một cách thê thảm </t>
+  </si>
+  <si>
+    <t>Được hưởng phúc, nhưng nên lập nghiệp ở nơi thật xa quê hương. Họ hàng khá giả, có danh giá và uy quyền tế thế, lại có nhiều người hiển đạt về võ nghiệp.</t>
+  </si>
+  <si>
+    <t>Không được hưởng phúc dồi dào, suốt đời may thường đi liền với rủi. Nên ly tổ có sớm xa gia đình mới mong được yên thân. Họ hàng khá giả, nhưng ly tán, có nhiều người hiển đạt về vỗ nghiệp</t>
+  </si>
+  <si>
+    <t>Bạc phúc nên giảm thọ. Khó tránh được lai nạn vẻ đao thương, dễ mắc hình ngục. Phải ly tổ, ở xa gia đình, may ra mới được yên thân. Họ hàng càng ngày càng sa sút, nghèo khổ, ly tán, lại có nhiều người chết
+non.</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Phúc Đức</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Họ hàng ly tán, thường lập nghiệp ở xa quê hương. </t>
+  </si>
+  <si>
+    <t>Được hưởng phúc, sống lâu, nhưng nên lập nghiệp
+ở nơi thật xa quê hương, Họ hàng khá giả. Tuy vậy ngành trưởng bao giờ cũng phiêu bạt, lụn bại.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Không được hưởng phúc dồi dào. Phải ly tán, sớm xa gia đình, mới mong được yên thân. Trong họ có người qúy hiển. </t>
+  </si>
+  <si>
+    <t>Bạc phúc nên giảm thọ. Khó tránh được tai họa. Phải ly tổ, sớm xa gia đình, may ra mới được yên thân. Họ hàng càng ngày càng sa sút.</t>
   </si>
 </sst>
 </file>
@@ -13312,227 +13397,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="47">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14059,10 +13924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4376"/>
+  <dimension ref="A1:B4378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3731" workbookViewId="0">
-      <selection activeCell="I3741" sqref="I3741"/>
+    <sheetView tabSelected="1" topLeftCell="A3726" workbookViewId="0">
+      <selection activeCell="C3733" sqref="C3733"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15683,7 +15548,7 @@
         <v>324</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>4402</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -16654,12 +16519,12 @@
         <v>445</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>446</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>446</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="325" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -16718,12 +16583,12 @@
         <v>453</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>454</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>454</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="333" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -16782,12 +16647,12 @@
         <v>461</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>462</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>462</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="341" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -16846,12 +16711,12 @@
         <v>469</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>470</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>470</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="349" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -16910,12 +16775,12 @@
         <v>477</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>478</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>478</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="357" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -16974,12 +16839,12 @@
         <v>485</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>486</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>486</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="365" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -17038,12 +16903,12 @@
         <v>493</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>494</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>494</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="373" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -17262,12 +17127,12 @@
         <v>521</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>522</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>522</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="401" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21246,12 +21111,12 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A898" s="1" t="s">
         <v>1013</v>
       </c>
       <c r="B898" s="1" t="s">
-        <v>1013</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="899" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21278,12 +21143,12 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="902" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A902" s="1" t="s">
         <v>1017</v>
       </c>
       <c r="B902" s="1" t="s">
-        <v>1017</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="903" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21310,12 +21175,12 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="906" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="906" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A906" s="1" t="s">
         <v>1021</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>1021</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="907" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21342,12 +21207,12 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A910" s="1" t="s">
         <v>1025</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>1025</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="911" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21374,12 +21239,12 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A914" s="1" t="s">
         <v>1029</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>1029</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="915" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21406,12 +21271,12 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A918" s="1" t="s">
         <v>1033</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>1033</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="919" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -21438,12 +21303,12 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A922" s="1" t="s">
         <v>1037</v>
       </c>
       <c r="B922" s="1" t="s">
-        <v>1037</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="923" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -23307,7 +23172,7 @@
         <v>1270</v>
       </c>
       <c r="B1155" s="1" t="s">
-        <v>4394</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="1156" spans="1:2" x14ac:dyDescent="0.25">
@@ -23323,7 +23188,7 @@
         <v>1272</v>
       </c>
       <c r="B1157" s="1" t="s">
-        <v>4395</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="1158" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -23934,12 +23799,12 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="1234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A1234" s="1" t="s">
         <v>1345</v>
       </c>
       <c r="B1234" s="1" t="s">
-        <v>1345</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="1235" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -24014,12 +23879,12 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="1244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1244" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1244" s="1" t="s">
         <v>1355</v>
       </c>
       <c r="B1244" s="1" t="s">
-        <v>1355</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="1245" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -24422,28 +24287,28 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="1295" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1295" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A1295" s="1" t="s">
         <v>1406</v>
       </c>
       <c r="B1295" s="1" t="s">
-        <v>1406</v>
-      </c>
-    </row>
-    <row r="1296" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A1296" s="1" t="s">
         <v>1407</v>
       </c>
       <c r="B1296" s="1" t="s">
-        <v>1407</v>
-      </c>
-    </row>
-    <row r="1297" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1297" s="1" t="s">
         <v>1408</v>
       </c>
       <c r="B1297" s="1" t="s">
-        <v>1408</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="1298" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -26406,12 +26271,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="1543" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1543" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A1543" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1543" s="1" t="s">
-        <v>22</v>
+        <v>4424</v>
       </c>
     </row>
     <row r="1544" spans="1:2" x14ac:dyDescent="0.25">
@@ -27046,12 +26911,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="1623" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1623" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1623" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B1623" s="1" t="s">
-        <v>96</v>
+        <v>4409</v>
       </c>
     </row>
     <row r="1624" spans="1:2" x14ac:dyDescent="0.25">
@@ -27240,10 +27105,10 @@
     </row>
     <row r="1647" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1647" s="1" t="s">
-        <v>4403</v>
+        <v>4401</v>
       </c>
       <c r="B1647" s="1" t="s">
-        <v>4404</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="1648" spans="1:2" x14ac:dyDescent="0.25">
@@ -33795,7 +33660,7 @@
         <v>2343</v>
       </c>
       <c r="B2466" s="1" t="s">
-        <v>4406</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="2467" spans="1:2" x14ac:dyDescent="0.25">
@@ -33803,7 +33668,7 @@
         <v>2344</v>
       </c>
       <c r="B2467" s="1" t="s">
-        <v>4406</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="2468" spans="1:2" x14ac:dyDescent="0.25">
@@ -33811,7 +33676,7 @@
         <v>2345</v>
       </c>
       <c r="B2468" s="1" t="s">
-        <v>4406</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="2469" spans="1:2" x14ac:dyDescent="0.25">
@@ -33843,7 +33708,7 @@
         <v>2349</v>
       </c>
       <c r="B2472" s="1" t="s">
-        <v>4405</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="2473" spans="1:2" x14ac:dyDescent="0.25">
@@ -33851,7 +33716,7 @@
         <v>2350</v>
       </c>
       <c r="B2473" s="1" t="s">
-        <v>4405</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="2474" spans="1:2" x14ac:dyDescent="0.25">
@@ -33859,7 +33724,7 @@
         <v>2351</v>
       </c>
       <c r="B2474" s="1" t="s">
-        <v>4405</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="2475" spans="1:2" x14ac:dyDescent="0.25">
@@ -33915,7 +33780,7 @@
         <v>2358</v>
       </c>
       <c r="B2481" s="1" t="s">
-        <v>4400</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="2482" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33923,7 +33788,7 @@
         <v>2359</v>
       </c>
       <c r="B2482" s="1" t="s">
-        <v>4400</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="2483" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33931,7 +33796,7 @@
         <v>2360</v>
       </c>
       <c r="B2483" s="1" t="s">
-        <v>4400</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="2484" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33939,7 +33804,7 @@
         <v>2361</v>
       </c>
       <c r="B2484" s="1" t="s">
-        <v>4400</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="2485" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33947,7 +33812,7 @@
         <v>2362</v>
       </c>
       <c r="B2485" s="1" t="s">
-        <v>4400</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="2486" spans="1:2" x14ac:dyDescent="0.25">
@@ -33963,7 +33828,7 @@
         <v>2364</v>
       </c>
       <c r="B2487" s="1" t="s">
-        <v>4401</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="2488" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -33971,7 +33836,7 @@
         <v>2365</v>
       </c>
       <c r="B2488" s="1" t="s">
-        <v>4401</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="2489" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -33979,7 +33844,7 @@
         <v>2366</v>
       </c>
       <c r="B2489" s="1" t="s">
-        <v>4401</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="2490" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -33987,7 +33852,7 @@
         <v>2367</v>
       </c>
       <c r="B2490" s="1" t="s">
-        <v>4401</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="2491" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -33995,7 +33860,7 @@
         <v>2368</v>
       </c>
       <c r="B2491" s="1" t="s">
-        <v>4401</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="2492" spans="1:2" x14ac:dyDescent="0.25">
@@ -34027,7 +33892,7 @@
         <v>2372</v>
       </c>
       <c r="B2495" s="1" t="s">
-        <v>4395</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="2496" spans="1:2" x14ac:dyDescent="0.25">
@@ -34075,7 +33940,7 @@
         <v>2378</v>
       </c>
       <c r="B2501" s="1" t="s">
-        <v>4395</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="2502" spans="1:2" x14ac:dyDescent="0.25">
@@ -34115,7 +33980,7 @@
         <v>2383</v>
       </c>
       <c r="B2506" s="1" t="s">
-        <v>4386</v>
+        <v>4384</v>
       </c>
     </row>
     <row r="2507" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -34123,7 +33988,7 @@
         <v>2384</v>
       </c>
       <c r="B2507" s="1" t="s">
-        <v>4389</v>
+        <v>4387</v>
       </c>
     </row>
     <row r="2508" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -34131,7 +33996,7 @@
         <v>2385</v>
       </c>
       <c r="B2508" s="1" t="s">
-        <v>4388</v>
+        <v>4386</v>
       </c>
     </row>
     <row r="2509" spans="1:2" x14ac:dyDescent="0.25">
@@ -34163,7 +34028,7 @@
         <v>2389</v>
       </c>
       <c r="B2512" s="1" t="s">
-        <v>4387</v>
+        <v>4385</v>
       </c>
     </row>
     <row r="2513" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -34171,7 +34036,7 @@
         <v>2390</v>
       </c>
       <c r="B2513" s="1" t="s">
-        <v>4389</v>
+        <v>4387</v>
       </c>
     </row>
     <row r="2514" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -34179,7 +34044,7 @@
         <v>2391</v>
       </c>
       <c r="B2514" s="1" t="s">
-        <v>4388</v>
+        <v>4386</v>
       </c>
     </row>
     <row r="2515" spans="1:2" x14ac:dyDescent="0.25">
@@ -34286,12 +34151,12 @@
         <v>2404</v>
       </c>
     </row>
-    <row r="2528" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2528" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2528" s="1" t="s">
         <v>2405</v>
       </c>
       <c r="B2528" s="1" t="s">
-        <v>2405</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="2529" spans="1:2" x14ac:dyDescent="0.25">
@@ -34302,12 +34167,12 @@
         <v>2406</v>
       </c>
     </row>
-    <row r="2530" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2530" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2530" s="1" t="s">
         <v>2407</v>
       </c>
       <c r="B2530" s="1" t="s">
-        <v>2407</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="2531" spans="1:2" x14ac:dyDescent="0.25">
@@ -34326,12 +34191,12 @@
         <v>2409</v>
       </c>
     </row>
-    <row r="2533" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2533" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2533" s="1" t="s">
         <v>2410</v>
       </c>
       <c r="B2533" s="1" t="s">
-        <v>2410</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="2534" spans="1:2" x14ac:dyDescent="0.25">
@@ -34342,12 +34207,12 @@
         <v>2411</v>
       </c>
     </row>
-    <row r="2535" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2535" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2535" s="1" t="s">
         <v>2412</v>
       </c>
       <c r="B2535" s="1" t="s">
-        <v>2412</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="2536" spans="1:2" x14ac:dyDescent="0.25">
@@ -34358,12 +34223,12 @@
         <v>2413</v>
       </c>
     </row>
-    <row r="2537" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2537" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2537" s="1" t="s">
         <v>2414</v>
       </c>
       <c r="B2537" s="1" t="s">
-        <v>2414</v>
+        <v>4409</v>
       </c>
     </row>
     <row r="2538" spans="1:2" x14ac:dyDescent="0.25">
@@ -34390,28 +34255,28 @@
         <v>2417</v>
       </c>
     </row>
-    <row r="2541" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2541" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2541" s="1" t="s">
         <v>2418</v>
       </c>
       <c r="B2541" s="1" t="s">
-        <v>2418</v>
-      </c>
-    </row>
-    <row r="2542" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4415</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2542" s="1" t="s">
         <v>2419</v>
       </c>
       <c r="B2542" s="1" t="s">
-        <v>2419</v>
-      </c>
-    </row>
-    <row r="2543" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4415</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2543" s="1" t="s">
         <v>2420</v>
       </c>
       <c r="B2543" s="1" t="s">
-        <v>2420</v>
+        <v>4415</v>
       </c>
     </row>
     <row r="2544" spans="1:2" x14ac:dyDescent="0.25">
@@ -34438,36 +34303,36 @@
         <v>2423</v>
       </c>
     </row>
-    <row r="2547" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2547" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2547" s="1" t="s">
         <v>2424</v>
       </c>
       <c r="B2547" s="1" t="s">
-        <v>2424</v>
-      </c>
-    </row>
-    <row r="2548" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2548" s="1" t="s">
         <v>2425</v>
       </c>
       <c r="B2548" s="1" t="s">
-        <v>2425</v>
-      </c>
-    </row>
-    <row r="2549" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2549" s="1" t="s">
         <v>2426</v>
       </c>
       <c r="B2549" s="1" t="s">
-        <v>2426</v>
-      </c>
-    </row>
-    <row r="2550" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2550" s="1" t="s">
         <v>2427</v>
       </c>
       <c r="B2550" s="1" t="s">
-        <v>2427</v>
+        <v>4418</v>
       </c>
     </row>
     <row r="2551" spans="1:2" x14ac:dyDescent="0.25">
@@ -34478,12 +34343,12 @@
         <v>2428</v>
       </c>
     </row>
-    <row r="2552" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2552" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2552" s="1" t="s">
         <v>2429</v>
       </c>
       <c r="B2552" s="1" t="s">
-        <v>2429</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="2553" spans="1:2" x14ac:dyDescent="0.25">
@@ -34494,12 +34359,12 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="2554" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2554" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2554" s="1" t="s">
         <v>2431</v>
       </c>
       <c r="B2554" s="1" t="s">
-        <v>2431</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="2555" spans="1:2" x14ac:dyDescent="0.25">
@@ -34510,12 +34375,12 @@
         <v>2432</v>
       </c>
     </row>
-    <row r="2556" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2556" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2556" s="1" t="s">
         <v>2433</v>
       </c>
       <c r="B2556" s="1" t="s">
-        <v>2433</v>
+        <v>4418</v>
       </c>
     </row>
     <row r="2557" spans="1:2" x14ac:dyDescent="0.25">
@@ -34526,12 +34391,12 @@
         <v>2434</v>
       </c>
     </row>
-    <row r="2558" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2558" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2558" s="1" t="s">
         <v>2435</v>
       </c>
       <c r="B2558" s="1" t="s">
-        <v>2435</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="2559" spans="1:2" x14ac:dyDescent="0.25">
@@ -34542,12 +34407,12 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="2560" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2560" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2560" s="1" t="s">
         <v>2437</v>
       </c>
       <c r="B2560" s="1" t="s">
-        <v>2437</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="2561" spans="1:2" x14ac:dyDescent="0.25">
@@ -34590,20 +34455,20 @@
         <v>2442</v>
       </c>
     </row>
-    <row r="2566" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2566" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2566" s="1" t="s">
         <v>2443</v>
       </c>
       <c r="B2566" s="1" t="s">
-        <v>2443</v>
-      </c>
-    </row>
-    <row r="2567" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2567" s="1" t="s">
         <v>2444</v>
       </c>
       <c r="B2567" s="1" t="s">
-        <v>2444</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="2568" spans="1:2" x14ac:dyDescent="0.25">
@@ -34638,36 +34503,36 @@
         <v>2448</v>
       </c>
     </row>
-    <row r="2572" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2572" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2572" s="1" t="s">
         <v>2449</v>
       </c>
       <c r="B2572" s="1" t="s">
-        <v>2449</v>
-      </c>
-    </row>
-    <row r="2573" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="2573" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2573" s="1" t="s">
         <v>2450</v>
       </c>
       <c r="B2573" s="1" t="s">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="2574" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2574" s="1" t="s">
         <v>2451</v>
       </c>
       <c r="B2574" s="1" t="s">
-        <v>2451</v>
-      </c>
-    </row>
-    <row r="2575" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2575" s="1" t="s">
         <v>2452</v>
       </c>
       <c r="B2575" s="1" t="s">
-        <v>2452</v>
+        <v>4423</v>
       </c>
     </row>
     <row r="2576" spans="1:2" x14ac:dyDescent="0.25">
@@ -34678,44 +34543,44 @@
         <v>2453</v>
       </c>
     </row>
-    <row r="2577" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2577" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2577" s="1" t="s">
         <v>2454</v>
       </c>
       <c r="B2577" s="1" t="s">
-        <v>2454</v>
-      </c>
-    </row>
-    <row r="2578" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4424</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2578" s="1" t="s">
         <v>2455</v>
       </c>
       <c r="B2578" s="1" t="s">
-        <v>2455</v>
-      </c>
-    </row>
-    <row r="2579" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2579" s="1" t="s">
         <v>2456</v>
       </c>
       <c r="B2579" s="1" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2580" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2580" s="1" t="s">
         <v>2457</v>
       </c>
       <c r="B2580" s="1" t="s">
-        <v>2457</v>
-      </c>
-    </row>
-    <row r="2581" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2581" s="1" t="s">
         <v>2458</v>
       </c>
       <c r="B2581" s="1" t="s">
-        <v>2458</v>
+        <v>4423</v>
       </c>
     </row>
     <row r="2582" spans="1:2" x14ac:dyDescent="0.25">
@@ -34726,28 +34591,28 @@
         <v>2459</v>
       </c>
     </row>
-    <row r="2583" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2583" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2583" s="1" t="s">
         <v>2460</v>
       </c>
       <c r="B2583" s="1" t="s">
-        <v>2460</v>
-      </c>
-    </row>
-    <row r="2584" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2584" s="1" t="s">
         <v>2461</v>
       </c>
       <c r="B2584" s="1" t="s">
-        <v>2461</v>
-      </c>
-    </row>
-    <row r="2585" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2585" s="1" t="s">
         <v>2462</v>
       </c>
       <c r="B2585" s="1" t="s">
-        <v>2462</v>
+        <v>4425</v>
       </c>
     </row>
     <row r="2586" spans="1:2" x14ac:dyDescent="0.25">
@@ -34755,7 +34620,7 @@
         <v>2463</v>
       </c>
       <c r="B2586" s="1" t="s">
-        <v>2463</v>
+        <v>4426</v>
       </c>
     </row>
     <row r="2587" spans="1:2" x14ac:dyDescent="0.25">
@@ -34782,20 +34647,20 @@
         <v>2466</v>
       </c>
     </row>
-    <row r="2590" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2590" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2590" s="1" t="s">
         <v>2467</v>
       </c>
       <c r="B2590" s="1" t="s">
-        <v>2467</v>
-      </c>
-    </row>
-    <row r="2591" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4427</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2591" s="1" t="s">
         <v>2468</v>
       </c>
       <c r="B2591" s="1" t="s">
-        <v>2468</v>
+        <v>4425</v>
       </c>
     </row>
     <row r="2592" spans="1:2" x14ac:dyDescent="0.25">
@@ -34803,7 +34668,7 @@
         <v>2469</v>
       </c>
       <c r="B2592" s="1" t="s">
-        <v>2469</v>
+        <v>4426</v>
       </c>
     </row>
     <row r="2593" spans="1:2" x14ac:dyDescent="0.25">
@@ -34830,20 +34695,20 @@
         <v>2472</v>
       </c>
     </row>
-    <row r="2596" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2596" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2596" s="1" t="s">
         <v>2473</v>
       </c>
       <c r="B2596" s="1" t="s">
-        <v>2473</v>
-      </c>
-    </row>
-    <row r="2597" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4427</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2597" s="1" t="s">
         <v>2474</v>
       </c>
       <c r="B2597" s="1" t="s">
-        <v>2474</v>
+        <v>4430</v>
       </c>
     </row>
     <row r="2598" spans="1:2" x14ac:dyDescent="0.25">
@@ -34854,12 +34719,12 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="2599" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2599" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2599" s="1" t="s">
         <v>2476</v>
       </c>
       <c r="B2599" s="1" t="s">
-        <v>2476</v>
+        <v>4429</v>
       </c>
     </row>
     <row r="2600" spans="1:2" x14ac:dyDescent="0.25">
@@ -34870,12 +34735,12 @@
         <v>2477</v>
       </c>
     </row>
-    <row r="2601" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2601" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2601" s="1" t="s">
         <v>2478</v>
       </c>
       <c r="B2601" s="1" t="s">
-        <v>2478</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="2602" spans="1:2" x14ac:dyDescent="0.25">
@@ -34886,12 +34751,12 @@
         <v>2479</v>
       </c>
     </row>
-    <row r="2603" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2603" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2603" s="1" t="s">
         <v>2480</v>
       </c>
       <c r="B2603" s="1" t="s">
-        <v>2480</v>
+        <v>4430</v>
       </c>
     </row>
     <row r="2604" spans="1:2" x14ac:dyDescent="0.25">
@@ -34902,12 +34767,12 @@
         <v>2481</v>
       </c>
     </row>
-    <row r="2605" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2605" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2605" s="1" t="s">
         <v>2482</v>
       </c>
       <c r="B2605" s="1" t="s">
-        <v>2482</v>
+        <v>4429</v>
       </c>
     </row>
     <row r="2606" spans="1:2" x14ac:dyDescent="0.25">
@@ -34918,12 +34783,12 @@
         <v>2483</v>
       </c>
     </row>
-    <row r="2607" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2607" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A2607" s="1" t="s">
         <v>2484</v>
       </c>
       <c r="B2607" s="1" t="s">
-        <v>2484</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="2608" spans="1:2" x14ac:dyDescent="0.25">
@@ -34934,12 +34799,12 @@
         <v>2485</v>
       </c>
     </row>
-    <row r="2609" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2609" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2609" s="1" t="s">
         <v>2486</v>
       </c>
       <c r="B2609" s="1" t="s">
-        <v>2486</v>
+        <v>4434</v>
       </c>
     </row>
     <row r="2610" spans="1:2" x14ac:dyDescent="0.25">
@@ -34950,12 +34815,12 @@
         <v>2487</v>
       </c>
     </row>
-    <row r="2611" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2611" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2611" s="1" t="s">
         <v>2488</v>
       </c>
       <c r="B2611" s="1" t="s">
-        <v>2488</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="2612" spans="1:2" x14ac:dyDescent="0.25">
@@ -34966,12 +34831,12 @@
         <v>2489</v>
       </c>
     </row>
-    <row r="2613" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2613" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2613" s="1" t="s">
         <v>2490</v>
       </c>
       <c r="B2613" s="1" t="s">
-        <v>2490</v>
+        <v>4435</v>
       </c>
     </row>
     <row r="2614" spans="1:2" x14ac:dyDescent="0.25">
@@ -34982,12 +34847,12 @@
         <v>2491</v>
       </c>
     </row>
-    <row r="2615" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2615" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2615" s="1" t="s">
         <v>2492</v>
       </c>
       <c r="B2615" s="1" t="s">
-        <v>2492</v>
+        <v>4434</v>
       </c>
     </row>
     <row r="2616" spans="1:2" x14ac:dyDescent="0.25">
@@ -34998,12 +34863,12 @@
         <v>2493</v>
       </c>
     </row>
-    <row r="2617" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2617" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2617" s="1" t="s">
         <v>2494</v>
       </c>
       <c r="B2617" s="1" t="s">
-        <v>2494</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="2618" spans="1:2" x14ac:dyDescent="0.25">
@@ -35014,12 +34879,12 @@
         <v>2495</v>
       </c>
     </row>
-    <row r="2619" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2619" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2619" s="1" t="s">
         <v>2496</v>
       </c>
       <c r="B2619" s="1" t="s">
-        <v>2496</v>
+        <v>4435</v>
       </c>
     </row>
     <row r="2620" spans="1:2" x14ac:dyDescent="0.25">
@@ -43846,12 +43711,12 @@
         <v>4379</v>
       </c>
     </row>
-    <row r="3723" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3723" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3723" s="1" t="s">
         <v>3721</v>
       </c>
       <c r="B3723" s="1" t="s">
-        <v>4381</v>
+        <v>4413</v>
       </c>
     </row>
     <row r="3724" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -43859,7 +43724,7 @@
         <v>3722</v>
       </c>
       <c r="B3724" s="1" t="s">
-        <v>4382</v>
+        <v>4381</v>
       </c>
     </row>
     <row r="3725" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -43867,7 +43732,7 @@
         <v>3723</v>
       </c>
       <c r="B3725" s="1" t="s">
-        <v>4385</v>
+        <v>4383</v>
       </c>
     </row>
     <row r="3726" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -43875,7 +43740,7 @@
         <v>3724</v>
       </c>
       <c r="B3726" s="1" t="s">
-        <v>4384</v>
+        <v>4419</v>
       </c>
     </row>
     <row r="3727" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -43883,7 +43748,7 @@
         <v>3725</v>
       </c>
       <c r="B3727" s="1" t="s">
-        <v>4383</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="3728" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -43891,7 +43756,7 @@
         <v>3726</v>
       </c>
       <c r="B3728" s="1" t="s">
-        <v>4391</v>
+        <v>4389</v>
       </c>
     </row>
     <row r="3729" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -43899,7 +43764,7 @@
         <v>3727</v>
       </c>
       <c r="B3729" s="1" t="s">
-        <v>4392</v>
+        <v>4390</v>
       </c>
     </row>
     <row r="3730" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -43907,7 +43772,7 @@
         <v>3728</v>
       </c>
       <c r="B3730" s="1" t="s">
-        <v>4393</v>
+        <v>4391</v>
       </c>
     </row>
     <row r="3731" spans="1:2" x14ac:dyDescent="0.25">
@@ -43915,7 +43780,7 @@
         <v>3729</v>
       </c>
       <c r="B3731" s="1" t="s">
-        <v>4396</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="3732" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -43923,7 +43788,7 @@
         <v>3730</v>
       </c>
       <c r="B3732" s="1" t="s">
-        <v>4397</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="3733" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -43931,7 +43796,7 @@
         <v>3731</v>
       </c>
       <c r="B3733" s="1" t="s">
-        <v>4398</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="3734" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -43939,7 +43804,7 @@
         <v>3732</v>
       </c>
       <c r="B3734" s="1" t="s">
-        <v>4399</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="3735" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -43947,7 +43812,7 @@
         <v>3733</v>
       </c>
       <c r="B3735" s="1" t="s">
-        <v>4407</v>
+        <v>4405</v>
       </c>
     </row>
     <row r="3736" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -43955,7 +43820,7 @@
         <v>3734</v>
       </c>
       <c r="B3736" s="1" t="s">
-        <v>4408</v>
+        <v>4406</v>
       </c>
     </row>
     <row r="3737" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -43963,7 +43828,7 @@
         <v>3735</v>
       </c>
       <c r="B3737" s="1" t="s">
-        <v>4409</v>
+        <v>4407</v>
       </c>
     </row>
     <row r="3738" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -43971,7 +43836,7 @@
         <v>3736</v>
       </c>
       <c r="B3738" s="1" t="s">
-        <v>4410</v>
+        <v>4408</v>
       </c>
     </row>
     <row r="3739" spans="1:2" x14ac:dyDescent="0.25">
@@ -49072,68 +48937,87 @@
     </row>
     <row r="4376" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A4376" s="1" t="s">
-        <v>4390</v>
+        <v>4388</v>
       </c>
       <c r="B4376" s="1" t="s">
-        <v>4389</v>
+        <v>4387</v>
+      </c>
+    </row>
+    <row r="4377" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4377" s="1" t="s">
+        <v>4411</v>
+      </c>
+      <c r="B4377" s="1" t="s">
+        <v>4412</v>
+      </c>
+    </row>
+    <row r="4378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4378" s="1" t="s">
+        <v>4432</v>
+      </c>
+      <c r="B4378" s="1" t="s">
+        <v>4433</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="23" priority="98"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="21" priority="68"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="19" priority="72"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="17" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6701:A1048576 A209:A1614 A1:A23 A25:A84 A143 A1788:A1792 A3425:A3830 A3893:A4167">
-    <cfRule type="duplicateValues" dxfId="16" priority="107"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="109"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="108"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="110"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1793:A3322">
-    <cfRule type="duplicateValues" dxfId="14" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3831:A3892">
-    <cfRule type="duplicateValues" dxfId="13" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4191:A4269">
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6701:B1048576 B209:B1614 B1:B23 B25:B84 B143 B1788:B1792 B3425:B3830 B3893:B4167">
-    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="13"/>
+  <conditionalFormatting sqref="B6701:B1048576 B1:B23 B25:B84 B143 B1788:B1792 B3425:B3830 B3893:B4167 B209:B1614">
+    <cfRule type="duplicateValues" dxfId="5" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1793:B3322">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3831:B3892">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1543">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Giải thích Phúc Đức
</commit_message>
<xml_diff>
--- a/LuanPhucDuc.xlsx
+++ b/LuanPhucDuc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F40207-970A-42F1-95AD-C551BF6219BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FEAE9F-1A81-4A77-AD85-664F78213462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6557" uniqueCount="3457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6561" uniqueCount="3465">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -10421,7 +10421,31 @@
     <t>Dòng họ nhiều người hiền lành, từ thiện, tốt tính, hay giúp đỡ, hỗ trợ nhau. Dòng họ mỗi người một nơi, mỗi người một xứ, không ở gần nhau.Ông bà tổ tiên mồ yên mả đẹp, nhiều người đã siêu thoát, không còn vấn vương, tái sinh cuộc sống khác.</t>
   </si>
   <si>
-    <t>Tổn thọ. Gia đình không toàn vẹn.</t>
+    <t>Tổn thọ. Gia đình không toàn vẹn.Ban phải chịu trách nhiệm chăm lo cho việc thờ cúng, mồ mả, có trách nhiệm và nghĩa vụ phải thờ cúng gia tiên, gánh vác các việc tâm linh liên quan đến gia đình.</t>
+  </si>
+  <si>
+    <t>Bạn cũng là người nhiều trách nhiệm, phải tự gây dựng, tôn bồi phúc đức nên phước đức riêng cho mình.</t>
+  </si>
+  <si>
+    <t>Trong dòng họ có nhiều người nghèo túng, bần hàn, phải tha hương lập nghiệp, hao hớt mỗi người một nơi, tìm về thì chẳng còn ai</t>
+  </si>
+  <si>
+    <t>Cũng là người được thừa hưởng phước đức tổ tiên, được may mắn về của tiền, người biết dùng của tiền làm phúc, tôn bồi phúc đức cho mình và dòng tộc.</t>
+  </si>
+  <si>
+    <t>Trong dòng họ nhiều người thành đạt, tuy nhiên dễ có bất đồng, cãi nhau trong việc thờ cúng, mồ mả tổ tiên.</t>
+  </si>
+  <si>
+    <t>Gia đình người hôn phối có chức quyền, khó tính, khắt khe, hay soi xét hoặc có người làm về ngành luật.</t>
+  </si>
+  <si>
+    <t>Trong dòng họ nhiều người tính toán, so đo, ngầm hại lẫn nhau. Gia đình người hôn phối nhiều mưu tính sau lưng mình.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dòng họ nhiều người có học thức, xuất phát từ dòng dõi nhà nho gia, có truyền thống học tốt. </t>
+  </si>
+  <si>
+    <t>Giúp tăng tuổi thọ, hưởng phúc, may mắn cho đương số. Dòng họ dễ có độc đinh, trong dòng họ có người mồ côi, có người mãi không chịu lấy vợ lấy chồng</t>
   </si>
 </sst>
 </file>
@@ -11145,8 +11169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A1:G3258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1591" workbookViewId="0">
-      <selection activeCell="C1598" sqref="C1598"/>
+    <sheetView tabSelected="1" topLeftCell="A1509" workbookViewId="0">
+      <selection activeCell="C1514" sqref="C1514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12519,7 +12543,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>192</v>
       </c>
@@ -12527,7 +12551,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>193</v>
       </c>
@@ -13743,7 +13767,7 @@
         <v>3374</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>345</v>
       </c>
@@ -13935,7 +13959,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>369</v>
       </c>
@@ -13999,7 +14023,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="356" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>377</v>
       </c>
@@ -14135,7 +14159,7 @@
         <v>3193</v>
       </c>
     </row>
-    <row r="373" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>394</v>
       </c>
@@ -14143,7 +14167,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>395</v>
       </c>
@@ -14351,7 +14375,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="400" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>421</v>
       </c>
@@ -18335,7 +18359,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="898" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A898" s="1" t="s">
         <v>912</v>
       </c>
@@ -18367,7 +18391,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="902" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A902" s="1" t="s">
         <v>916</v>
       </c>
@@ -18463,7 +18487,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="914" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A914" s="1" t="s">
         <v>928</v>
       </c>
@@ -18495,7 +18519,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="918" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A918" s="1" t="s">
         <v>932</v>
       </c>
@@ -21103,7 +21127,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="1244" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1244" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1244" s="1" t="s">
         <v>1254</v>
       </c>
@@ -21527,7 +21551,7 @@
         <v>3222</v>
       </c>
     </row>
-    <row r="1297" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1297" s="1" t="s">
         <v>1307</v>
       </c>
@@ -23247,12 +23271,12 @@
         <v>3267</v>
       </c>
     </row>
-    <row r="1512" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1512" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A1512" s="1" t="s">
         <v>1522</v>
       </c>
       <c r="B1512" s="1" t="s">
-        <v>1522</v>
+        <v>3464</v>
       </c>
     </row>
     <row r="1513" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -23652,7 +23676,7 @@
         <v>3396</v>
       </c>
     </row>
-    <row r="1560" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="1560" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A1560" s="1" t="s">
         <v>1557</v>
       </c>
@@ -23798,7 +23822,7 @@
         <v>3417</v>
       </c>
     </row>
-    <row r="1576" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="1576" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A1576" s="1" t="s">
         <v>1573</v>
       </c>
@@ -23994,52 +24018,64 @@
         <v>3455</v>
       </c>
     </row>
-    <row r="1594" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1594" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A1594" s="1" t="s">
         <v>1590</v>
       </c>
       <c r="B1594" s="1" t="s">
         <v>3456</v>
       </c>
-    </row>
-    <row r="1595" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C1594" s="1" t="s">
+        <v>3457</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A1595" s="1" t="s">
         <v>2847</v>
       </c>
       <c r="B1595" s="1" t="s">
-        <v>2847</v>
-      </c>
-    </row>
-    <row r="1596" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3458</v>
+      </c>
+      <c r="C1595" s="1" t="s">
+        <v>3459</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A1596" s="1" t="s">
         <v>2848</v>
       </c>
       <c r="B1596" s="1" t="s">
-        <v>2848</v>
-      </c>
-    </row>
-    <row r="1597" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3458</v>
+      </c>
+      <c r="C1596" s="1" t="s">
+        <v>3459</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1597" s="1" t="s">
         <v>1593</v>
       </c>
       <c r="B1597" s="1" t="s">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="1598" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3460</v>
+      </c>
+      <c r="C1597" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1598" s="1" t="s">
         <v>1592</v>
       </c>
       <c r="B1598" s="1" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="1599" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3462</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1599" s="1" t="s">
         <v>2849</v>
       </c>
       <c r="B1599" s="1" t="s">
-        <v>2849</v>
+        <v>3463</v>
       </c>
     </row>
     <row r="1600" spans="1:7" x14ac:dyDescent="0.25">
@@ -24306,7 +24342,7 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="1633" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1633" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1633" s="1" t="s">
         <v>1620</v>
       </c>
@@ -24314,7 +24350,7 @@
         <v>3192</v>
       </c>
     </row>
-    <row r="1634" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1634" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1634" s="1" t="s">
         <v>1621</v>
       </c>
@@ -24322,7 +24358,7 @@
         <v>3192</v>
       </c>
     </row>
-    <row r="1635" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1635" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1635" s="1" t="s">
         <v>1622</v>
       </c>
@@ -24330,7 +24366,7 @@
         <v>3192</v>
       </c>
     </row>
-    <row r="1636" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1636" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1636" s="1" t="s">
         <v>1623</v>
       </c>
@@ -24338,7 +24374,7 @@
         <v>3192</v>
       </c>
     </row>
-    <row r="1637" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1637" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1637" s="1" t="s">
         <v>1624</v>
       </c>
@@ -37347,97 +37383,87 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="39" priority="114"/>
-    <cfRule type="duplicateValues" dxfId="38" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="115"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="114"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="37" priority="84"/>
-    <cfRule type="duplicateValues" dxfId="36" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="84"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="35" priority="88"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
     <cfRule type="duplicateValues" dxfId="33" priority="83"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A1559:A1585 A1587:A2474">
+    <cfRule type="duplicateValues" dxfId="32" priority="2102"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2957:A2961">
-    <cfRule type="duplicateValues" dxfId="32" priority="1158"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1158"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2987:A3065">
-    <cfRule type="duplicateValues" dxfId="31" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5496:A1048576 A209:A1541 A1:A23 A25:A84 A143 A2577:A2956 A2962:A2983">
-    <cfRule type="duplicateValues" dxfId="30" priority="123"/>
     <cfRule type="duplicateValues" dxfId="29" priority="125"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="123"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1586:B1586">
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3258:B1048576 A3254:A3257 A1:B1584 A1585 A1587:B3253">
-    <cfRule type="duplicateValues" dxfId="28" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="26" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="24" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="22" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B234">
-    <cfRule type="duplicateValues" dxfId="19" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1534">
-    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2957:B2961">
-    <cfRule type="duplicateValues" dxfId="17" priority="1159"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5496:B1048576 B1:B23 B143 B2962:B2983 B2577:B2956 B25:B84 B209:B1541">
-    <cfRule type="duplicateValues" dxfId="16" priority="28"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1559:A1585 A1587:A2474">
-    <cfRule type="duplicateValues" dxfId="14" priority="2102"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1559:B1584 B1587:B2474">
     <cfRule type="duplicateValues" dxfId="13" priority="2104"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2969">
-    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+  <conditionalFormatting sqref="B1585">
+    <cfRule type="duplicateValues" dxfId="12" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2957:B2961">
+    <cfRule type="duplicateValues" dxfId="9" priority="1159"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2985">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5496:B1048576 B1:B23 B143 B2962:B2983 B2577:B2956 B25:B84 B209:B1541">
+    <cfRule type="duplicateValues" dxfId="6" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2969">
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2985">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1585">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1585">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1585">
-    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1586:B1586">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1586:B1586">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1586:B1586">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1586:W1586">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>

</xml_diff>